<commit_message>
updates to intro screens
</commit_message>
<xml_diff>
--- a/documents/article/Polarization Measures.xlsx
+++ b/documents/article/Polarization Measures.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameshoughton/Google Drive/MIT PhD/Factionalism_Research/detective-game-interdependent-diffusion/documents/article/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97E5DDA-6EDE-6943-B11A-95FC7DB7F405}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56298433-B2E5-984C-8F14-E6D8467E46CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11000" yWindow="-21600" windowWidth="24840" windowHeight="21600" activeTab="1" xr2:uid="{F01117A4-CCCF-B543-9FAF-5B1A22C76FCE}"/>
+    <workbookView xWindow="16080" yWindow="-18180" windowWidth="24840" windowHeight="17540" activeTab="1" xr2:uid="{F01117A4-CCCF-B543-9FAF-5B1A22C76FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -653,7 +654,7 @@
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
@@ -733,7 +734,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>